<commit_message>
Equipamiento de inicio del labor
</commit_message>
<xml_diff>
--- a/Actividades/Taller01006/Presupuestos.xlsx
+++ b/Actividades/Taller01006/Presupuestos.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkfm\pf\proyectofinal2019\Actividades\Taller01006\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEF8CAB-5117-4137-8F9F-EE91BF5677EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="36">
   <si>
     <t>Presupuestos:</t>
   </si>
@@ -135,12 +134,15 @@
   </si>
   <si>
     <t>PESOS</t>
+  </si>
+  <si>
+    <t>Red Hat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -485,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -804,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <f>D27*E27</f>
+        <f t="shared" ref="F27:F32" si="1">D27*E27</f>
         <v>1293</v>
       </c>
       <c r="G27" t="s">
@@ -822,7 +824,7 @@
         <v>3</v>
       </c>
       <c r="F28">
-        <f>D28*E28</f>
+        <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="G28" t="s">
@@ -840,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="F29">
-        <f>D29*E29</f>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="G29" t="s">
@@ -858,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <f>D30*E30</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="G30" t="s">
@@ -876,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <f>D31*E31</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="G31" t="s">
@@ -894,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <f>D32*E32</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="G32" t="s">
@@ -1147,7 +1149,7 @@
         <v>8</v>
       </c>
       <c r="F57">
-        <f t="shared" ref="F57:F62" si="1">D57*E57</f>
+        <f t="shared" ref="F57:F62" si="2">D57*E57</f>
         <v>2856</v>
       </c>
       <c r="G57" t="s">
@@ -1165,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2448</v>
       </c>
       <c r="G58" t="s">
@@ -1183,7 +1185,7 @@
         <v>19</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2033</v>
       </c>
       <c r="G59" t="s">
@@ -1201,7 +1203,7 @@
         <v>2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>390</v>
       </c>
       <c r="G60" t="s">
@@ -1219,7 +1221,7 @@
         <v>124</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1240</v>
       </c>
       <c r="G61" t="s">
@@ -1237,7 +1239,7 @@
         <v>16</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2160</v>
       </c>
       <c r="G62" t="s">
@@ -1260,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="F65">
-        <f>D65*E65</f>
+        <f t="shared" ref="F65:F70" si="3">D65*E65</f>
         <v>6100</v>
       </c>
       <c r="G65" t="s">
@@ -1278,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="F66">
-        <f>D66*E66</f>
+        <f t="shared" si="3"/>
         <v>870</v>
       </c>
       <c r="G66" t="s">
@@ -1296,7 +1298,7 @@
         <v>2</v>
       </c>
       <c r="F67">
-        <f>D67*E67</f>
+        <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="G67" t="s">
@@ -1314,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <f>D68*E68</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="G68" t="s">
@@ -1332,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <f>D69*E69</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="G69" t="s">
@@ -1350,7 +1352,7 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <f>D70*E70</f>
+        <f t="shared" si="3"/>
         <v>826</v>
       </c>
       <c r="G70" t="s">
@@ -1621,7 +1623,7 @@
         <v>8</v>
       </c>
       <c r="F95">
-        <f t="shared" ref="F95:F100" si="2">D95*E95</f>
+        <f t="shared" ref="F95:F100" si="4">D95*E95</f>
         <v>2856</v>
       </c>
       <c r="G95" t="s">
@@ -1639,7 +1641,7 @@
         <v>8</v>
       </c>
       <c r="F96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2448</v>
       </c>
       <c r="G96" t="s">
@@ -1657,7 +1659,7 @@
         <v>19</v>
       </c>
       <c r="F97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9044</v>
       </c>
       <c r="G97" t="s">
@@ -1675,7 +1677,7 @@
         <v>2</v>
       </c>
       <c r="F98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>516</v>
       </c>
       <c r="G98" t="s">
@@ -1693,7 +1695,7 @@
         <v>124</v>
       </c>
       <c r="F99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1240</v>
       </c>
       <c r="G99" t="s">
@@ -1711,7 +1713,7 @@
         <v>16</v>
       </c>
       <c r="F100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2160</v>
       </c>
       <c r="G100" t="s">
@@ -1734,7 +1736,7 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <f>D103*E103</f>
+        <f t="shared" ref="F103:F108" si="5">D103*E103</f>
         <v>6100</v>
       </c>
       <c r="G103" t="s">
@@ -1752,7 +1754,7 @@
         <v>3</v>
       </c>
       <c r="F104">
-        <f>D104*E104</f>
+        <f t="shared" si="5"/>
         <v>870</v>
       </c>
       <c r="G104" t="s">
@@ -1770,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="F105">
-        <f>D105*E105</f>
+        <f t="shared" si="5"/>
         <v>297</v>
       </c>
       <c r="G105" t="s">
@@ -1788,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="F106">
-        <f>D106*E106</f>
+        <f t="shared" si="5"/>
         <v>125</v>
       </c>
       <c r="G106" t="s">
@@ -1806,7 +1808,7 @@
         <v>1</v>
       </c>
       <c r="F107">
-        <f>D107*E107</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="G107" t="s">
@@ -1824,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="F108">
-        <f>D108*E108</f>
+        <f t="shared" si="5"/>
         <v>826</v>
       </c>
       <c r="G108" t="s">
@@ -1869,6 +1871,24 @@
         <v>8000</v>
       </c>
       <c r="G112" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>35</v>
+      </c>
+      <c r="D113">
+        <v>349</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="F113">
+        <f>D113*E113</f>
+        <v>349</v>
+      </c>
+      <c r="G113" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subo lo de taller arreglado y la just de SO
</commit_message>
<xml_diff>
--- a/Actividades/Taller01006/Presupuestos.xlsx
+++ b/Actividades/Taller01006/Presupuestos.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkfm\pf\proyectofinal2019\Actividades\Taller01006\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Downloads\Taller\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C11B092-41AB-45A2-BC32-8F8F32D5411D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="38">
   <si>
     <t>Presupuestos:</t>
   </si>
@@ -140,12 +141,15 @@
   </si>
   <si>
     <t>Precio (Moneda)</t>
+  </si>
+  <si>
+    <t>Patchera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,14 +494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
@@ -536,8 +540,8 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f ca="1">SUM(F6:F36)</f>
-        <v>56172.43</v>
+        <f ca="1">SUM(F6:F37)</f>
+        <v>57667.43</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -757,11 +761,11 @@
         <v>195</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="3"/>
-        <v>390</v>
+        <v>585</v>
       </c>
       <c r="G22" t="s">
         <v>28</v>
@@ -957,13 +961,30 @@
         <v>28</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <v>1300</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1300</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>8</v>
       </c>
       <c r="B39">
-        <f ca="1">SUM(F42:F74)</f>
-        <v>90544.43</v>
+        <f ca="1">SUM(F42:F76)</f>
+        <v>92759.43</v>
       </c>
       <c r="C39" t="s">
         <v>28</v>
@@ -1213,11 +1234,11 @@
         <v>195</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60">
         <f t="shared" ca="1" si="9"/>
-        <v>390</v>
+        <v>585</v>
       </c>
       <c r="G60" t="s">
         <v>28</v>
@@ -1259,649 +1280,702 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63">
+        <v>90</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63">
+        <f>D63*E63</f>
+        <v>720</v>
+      </c>
+      <c r="G63" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65">
-        <v>6100</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <f t="shared" ref="F65:F70" ca="1" si="10">ROUND((D65*E65)/VLOOKUP(G65, INDIRECT("K2:L3"), 2),2)</f>
-        <v>6100</v>
-      </c>
-      <c r="G65" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>6100</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="F66:F71" ca="1" si="10">ROUND((D66*E66)/VLOOKUP(G66, INDIRECT("K2:L3"), 2),2)</f>
+        <v>6100</v>
+      </c>
+      <c r="G66" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>13</v>
       </c>
-      <c r="D66">
+      <c r="D67">
         <v>290</v>
       </c>
-      <c r="E66">
+      <c r="E67">
         <v>3</v>
       </c>
-      <c r="F66">
+      <c r="F67">
         <f t="shared" ca="1" si="10"/>
         <v>870</v>
       </c>
-      <c r="G66" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
+      <c r="G67" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>29</v>
       </c>
-      <c r="D67">
+      <c r="D68">
         <v>99</v>
       </c>
-      <c r="E67">
+      <c r="E68">
         <v>2</v>
       </c>
-      <c r="F67">
+      <c r="F68">
         <f t="shared" ca="1" si="10"/>
         <v>198</v>
       </c>
-      <c r="G67" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+      <c r="G68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>11</v>
       </c>
-      <c r="D68">
+      <c r="D69">
         <v>125</v>
       </c>
-      <c r="E68">
+      <c r="E69">
         <v>1</v>
       </c>
-      <c r="F68">
+      <c r="F69">
         <f t="shared" ca="1" si="10"/>
         <v>125</v>
       </c>
-      <c r="G68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
+      <c r="G69" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>30</v>
       </c>
-      <c r="D69">
+      <c r="D70">
         <v>13</v>
       </c>
-      <c r="E69">
+      <c r="E70">
         <v>1</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <f t="shared" ca="1" si="10"/>
         <v>13</v>
       </c>
-      <c r="G69" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
+      <c r="G70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>22</v>
       </c>
-      <c r="D70">
+      <c r="D71">
         <v>826</v>
       </c>
-      <c r="E70">
+      <c r="E71">
         <v>1</v>
       </c>
-      <c r="F70">
+      <c r="F71">
         <f t="shared" ca="1" si="10"/>
         <v>826</v>
       </c>
-      <c r="G70" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="G71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D73">
-        <v>235</v>
-      </c>
-      <c r="E73">
-        <v>40</v>
-      </c>
-      <c r="F73">
-        <f t="shared" ref="F73:F74" ca="1" si="11">ROUND((D73*E73)/VLOOKUP(G73, INDIRECT("K2:L3"), 2),2)</f>
-        <v>9400</v>
-      </c>
-      <c r="G73" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74">
+        <v>235</v>
+      </c>
+      <c r="E74">
+        <v>40</v>
+      </c>
+      <c r="F74">
+        <f t="shared" ref="F74:F75" ca="1" si="11">ROUND((D74*E74)/VLOOKUP(G74, INDIRECT("K2:L3"), 2),2)</f>
+        <v>9400</v>
+      </c>
+      <c r="G74" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>24</v>
       </c>
-      <c r="D74">
+      <c r="D75">
         <v>4000</v>
       </c>
-      <c r="E74">
+      <c r="E75">
         <v>1</v>
       </c>
-      <c r="F74">
+      <c r="F75">
         <f t="shared" ca="1" si="11"/>
         <v>4000</v>
       </c>
-      <c r="G74" t="s">
+      <c r="G75" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="C76" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76">
+        <v>1300</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <v>1300</v>
+      </c>
+      <c r="G76" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>9</v>
       </c>
-      <c r="B76">
-        <f ca="1">SUM(F79:F112)</f>
-        <v>143354.43</v>
-      </c>
-      <c r="C76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="B78">
+        <f ca="1">SUM(F81:F116)</f>
+        <v>145632.43</v>
+      </c>
+      <c r="C78" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>10</v>
       </c>
-      <c r="D79">
+      <c r="D81">
         <v>530</v>
       </c>
-      <c r="E79">
+      <c r="E81">
         <v>30</v>
       </c>
-      <c r="F79">
-        <f t="shared" ref="F79:F82" ca="1" si="12">ROUND((D79*E79)/VLOOKUP(G79, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F81">
+        <f t="shared" ref="F81:F84" ca="1" si="12">ROUND((D81*E81)/VLOOKUP(G81, INDIRECT("K2:L3"), 2),2)</f>
         <v>15900</v>
       </c>
-      <c r="G79" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+      <c r="G81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
         <v>11</v>
       </c>
-      <c r="D80">
+      <c r="D82">
         <v>125</v>
       </c>
-      <c r="E80">
+      <c r="E82">
         <v>30</v>
       </c>
-      <c r="F80">
+      <c r="F82">
         <f t="shared" ca="1" si="12"/>
         <v>3750</v>
       </c>
-      <c r="G80" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+      <c r="G82" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
         <v>12</v>
       </c>
-      <c r="D81">
+      <c r="D83">
         <v>21</v>
       </c>
-      <c r="E81">
+      <c r="E83">
         <v>30</v>
       </c>
-      <c r="F81">
+      <c r="F83">
         <f t="shared" ca="1" si="12"/>
         <v>630</v>
       </c>
-      <c r="G81" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+      <c r="G83" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
         <v>13</v>
       </c>
-      <c r="D82">
+      <c r="D84">
         <v>66</v>
       </c>
-      <c r="E82">
+      <c r="E84">
         <v>30</v>
       </c>
-      <c r="F82">
+      <c r="F84">
         <f t="shared" ca="1" si="12"/>
         <v>1980</v>
       </c>
-      <c r="G82" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="G84" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>15</v>
       </c>
-      <c r="D85">
+      <c r="D87">
         <v>475</v>
       </c>
-      <c r="E85">
+      <c r="E87">
         <v>10</v>
       </c>
-      <c r="F85">
-        <f t="shared" ref="F85:F88" ca="1" si="13">ROUND((D85*E85)/VLOOKUP(G85, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F87">
+        <f t="shared" ref="F87:F90" ca="1" si="13">ROUND((D87*E87)/VLOOKUP(G87, INDIRECT("K2:L3"), 2),2)</f>
         <v>4750</v>
       </c>
-      <c r="G85" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
+      <c r="G87" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>16</v>
       </c>
-      <c r="D86">
+      <c r="D88">
         <v>1607</v>
       </c>
-      <c r="E86">
+      <c r="E88">
         <v>20</v>
       </c>
-      <c r="F86">
+      <c r="F88">
         <f t="shared" ca="1" si="13"/>
         <v>32140</v>
       </c>
-      <c r="G86" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
+      <c r="G88" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>11</v>
       </c>
-      <c r="D87">
+      <c r="D89">
         <v>125</v>
       </c>
-      <c r="E87">
+      <c r="E89">
         <v>10</v>
       </c>
-      <c r="F87">
+      <c r="F89">
         <f t="shared" ca="1" si="13"/>
         <v>1250</v>
       </c>
-      <c r="G87" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+      <c r="G89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>12</v>
       </c>
-      <c r="D88">
+      <c r="D90">
         <v>21</v>
       </c>
-      <c r="E88">
+      <c r="E90">
         <v>10</v>
       </c>
-      <c r="F88">
+      <c r="F90">
         <f t="shared" ca="1" si="13"/>
         <v>210</v>
       </c>
-      <c r="G88" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+      <c r="G90" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C91" t="s">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>10</v>
       </c>
-      <c r="D91">
+      <c r="D93">
         <v>1607</v>
       </c>
-      <c r="E91">
+      <c r="E93">
         <v>20</v>
       </c>
-      <c r="F91">
-        <f t="shared" ref="F91:F92" ca="1" si="14">ROUND((D91*E91)/VLOOKUP(G91, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F93">
+        <f t="shared" ref="F93:F94" ca="1" si="14">ROUND((D93*E93)/VLOOKUP(G93, INDIRECT("K2:L3"), 2),2)</f>
         <v>32140</v>
       </c>
-      <c r="G91" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C92" t="s">
+      <c r="G93" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>17</v>
       </c>
-      <c r="D92">
+      <c r="D94">
         <v>395</v>
       </c>
-      <c r="E92">
+      <c r="E94">
         <v>20</v>
       </c>
-      <c r="F92">
+      <c r="F94">
         <f t="shared" ca="1" si="14"/>
         <v>7900</v>
       </c>
-      <c r="G92" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="G94" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
         <v>18</v>
       </c>
-      <c r="D95">
+      <c r="D97">
         <v>357</v>
       </c>
-      <c r="E95">
+      <c r="E97">
         <v>8</v>
       </c>
-      <c r="F95">
-        <f t="shared" ref="F95:F100" ca="1" si="15">ROUND((D95*E95)/VLOOKUP(G95, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F97">
+        <f t="shared" ref="F97:F102" ca="1" si="15">ROUND((D97*E97)/VLOOKUP(G97, INDIRECT("K2:L3"), 2),2)</f>
         <v>2856</v>
       </c>
-      <c r="G95" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
+      <c r="G97" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
         <v>19</v>
       </c>
-      <c r="D96">
+      <c r="D98">
         <v>306</v>
       </c>
-      <c r="E96">
+      <c r="E98">
         <v>8</v>
       </c>
-      <c r="F96">
+      <c r="F98">
         <f t="shared" ca="1" si="15"/>
         <v>2448</v>
       </c>
-      <c r="G96" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C97" t="s">
+      <c r="G98" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>20</v>
       </c>
-      <c r="D97">
+      <c r="D99">
         <v>476</v>
       </c>
-      <c r="E97">
+      <c r="E99">
         <v>19</v>
       </c>
-      <c r="F97">
+      <c r="F99">
         <f t="shared" ca="1" si="15"/>
         <v>9044</v>
       </c>
-      <c r="G97" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
+      <c r="G99" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>21</v>
       </c>
-      <c r="D98">
+      <c r="D100">
         <v>258</v>
       </c>
-      <c r="E98">
-        <v>2</v>
-      </c>
-      <c r="F98">
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100">
         <f t="shared" ca="1" si="15"/>
-        <v>516</v>
-      </c>
-      <c r="G98" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
+        <v>774</v>
+      </c>
+      <c r="G100" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
         <v>31</v>
       </c>
-      <c r="D99">
+      <c r="D101">
         <v>10</v>
       </c>
-      <c r="E99">
+      <c r="E101">
         <v>124</v>
       </c>
-      <c r="F99">
+      <c r="F101">
         <f t="shared" ca="1" si="15"/>
         <v>35.43</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G101" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
         <v>22</v>
       </c>
-      <c r="D100">
+      <c r="D102">
         <v>135</v>
       </c>
-      <c r="E100">
+      <c r="E102">
         <v>16</v>
       </c>
-      <c r="F100">
+      <c r="F102">
         <f t="shared" ca="1" si="15"/>
         <v>2160</v>
       </c>
-      <c r="G100" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>6</v>
+      <c r="G102" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C103" t="s">
+        <v>37</v>
+      </c>
+      <c r="D103">
+        <v>90</v>
+      </c>
+      <c r="E103">
+        <v>8</v>
+      </c>
+      <c r="F103">
+        <f>D103*E103</f>
+        <v>720</v>
+      </c>
+      <c r="G103" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
         <v>6</v>
       </c>
-      <c r="D103">
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106">
         <v>6100</v>
       </c>
-      <c r="E103">
+      <c r="E106">
         <v>1</v>
       </c>
-      <c r="F103">
-        <f t="shared" ref="F103:F108" ca="1" si="16">ROUND((D103*E103)/VLOOKUP(G103, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F106">
+        <f t="shared" ref="F106:F111" ca="1" si="16">ROUND((D106*E106)/VLOOKUP(G106, INDIRECT("K2:L3"), 2),2)</f>
         <v>6100</v>
       </c>
-      <c r="G103" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+      <c r="G106" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>13</v>
       </c>
-      <c r="D104">
+      <c r="D107">
         <v>290</v>
       </c>
-      <c r="E104">
+      <c r="E107">
         <v>3</v>
       </c>
-      <c r="F104">
+      <c r="F107">
         <f t="shared" ca="1" si="16"/>
         <v>870</v>
       </c>
-      <c r="G104" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
+      <c r="G107" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
         <v>29</v>
       </c>
-      <c r="D105">
+      <c r="D108">
         <v>99</v>
       </c>
-      <c r="E105">
+      <c r="E108">
         <v>3</v>
       </c>
-      <c r="F105">
+      <c r="F108">
         <f t="shared" ca="1" si="16"/>
         <v>297</v>
       </c>
-      <c r="G105" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C106" t="s">
+      <c r="G108" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>11</v>
       </c>
-      <c r="D106">
+      <c r="D109">
         <v>125</v>
       </c>
-      <c r="E106">
+      <c r="E109">
         <v>1</v>
       </c>
-      <c r="F106">
+      <c r="F109">
         <f t="shared" ca="1" si="16"/>
         <v>125</v>
       </c>
-      <c r="G106" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+      <c r="G109" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
         <v>30</v>
       </c>
-      <c r="D107">
+      <c r="D110">
         <v>27</v>
       </c>
-      <c r="E107">
+      <c r="E110">
         <v>1</v>
       </c>
-      <c r="F107">
+      <c r="F110">
         <f t="shared" ca="1" si="16"/>
         <v>27</v>
       </c>
-      <c r="G107" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C108" t="s">
+      <c r="G110" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
         <v>22</v>
       </c>
-      <c r="D108">
+      <c r="D111">
         <v>826</v>
       </c>
-      <c r="E108">
+      <c r="E111">
         <v>1</v>
       </c>
-      <c r="F108">
+      <c r="F111">
         <f t="shared" ca="1" si="16"/>
         <v>826</v>
       </c>
-      <c r="G108" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+      <c r="G111" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C111" t="s">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
         <v>23</v>
       </c>
-      <c r="D111">
+      <c r="D114">
         <v>235</v>
       </c>
-      <c r="E111">
+      <c r="E114">
         <v>40</v>
       </c>
-      <c r="F111">
-        <f t="shared" ref="F111:F113" ca="1" si="17">ROUND((D111*E111)/VLOOKUP(G111, INDIRECT("K2:L3"), 2),2)</f>
+      <c r="F114">
+        <f t="shared" ref="F114:F116" ca="1" si="17">ROUND((D114*E114)/VLOOKUP(G114, INDIRECT("K2:L3"), 2),2)</f>
         <v>9400</v>
       </c>
-      <c r="G111" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C112" t="s">
+      <c r="G114" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
         <v>24</v>
       </c>
-      <c r="D112">
+      <c r="D115">
         <v>8000</v>
       </c>
-      <c r="E112">
+      <c r="E115">
         <v>1</v>
       </c>
-      <c r="F112">
+      <c r="F115">
         <f t="shared" ca="1" si="17"/>
         <v>8000</v>
       </c>
-      <c r="G112" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="113" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C113" t="s">
+      <c r="G115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
         <v>33</v>
       </c>
-      <c r="D113">
-        <v>349</v>
-      </c>
-      <c r="E113">
+      <c r="D116">
+        <v>1300</v>
+      </c>
+      <c r="E116">
         <v>1</v>
       </c>
-      <c r="F113">
+      <c r="F116">
         <f t="shared" ca="1" si="17"/>
-        <v>349</v>
-      </c>
-      <c r="G113" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G116" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Subo todos los presupuestos en publisher
</commit_message>
<xml_diff>
--- a/Actividades/Taller01006/Presupuestos.xlsx
+++ b/Actividades/Taller01006/Presupuestos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Downloads\Taller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\Leonardo\proyectofinal2019\Actividades\Taller01006\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABAAC67-17F8-42C5-A264-05306291E52D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B114AB4B-A676-4F27-B121-A82ABDFBC081}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10365" yWindow="15" windowWidth="10140" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="48">
   <si>
     <t>Presupuestos:</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Ficha</t>
   </si>
   <si>
-    <t>PESOS</t>
-  </si>
-  <si>
     <t>Red Hat</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Impresora</t>
+  </si>
+  <si>
+    <t>0.3</t>
   </si>
 </sst>
 </file>
@@ -209,8 +209,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,13 +545,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
         <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
         <v>26</v>
@@ -559,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2">
         <v>35</v>
@@ -571,7 +574,7 @@
       </c>
       <c r="B3">
         <f ca="1">SUM(F6:F49)</f>
-        <v>70067</v>
+        <v>68568</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -626,7 +629,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>54</v>
@@ -803,7 +806,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>258</v>
@@ -821,7 +824,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <v>305</v>
@@ -839,7 +842,7 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25">
         <v>87</v>
@@ -857,7 +860,7 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26">
         <v>99</v>
@@ -877,18 +880,17 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D27">
-        <v>10</v>
+      <c r="D27" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E27">
         <v>154</v>
       </c>
       <c r="F27">
-        <f>PRODUCT(D27*E27)</f>
-        <v>1540</v>
+        <v>41</v>
       </c>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -911,7 +913,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29">
         <v>6</v>
@@ -929,7 +931,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -947,7 +949,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -988,7 +990,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35">
         <v>1293</v>
@@ -1006,7 +1008,7 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36">
         <v>1293</v>
@@ -1042,7 +1044,7 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D38">
         <v>449</v>
@@ -1060,7 +1062,7 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39">
         <v>449</v>
@@ -1209,7 +1211,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D49">
         <v>1300</v>
@@ -1230,7 +1232,7 @@
       </c>
       <c r="B51">
         <f ca="1">SUM(F54:F98)</f>
-        <v>113926</v>
+        <v>112427</v>
       </c>
       <c r="C51" t="s">
         <v>27</v>
@@ -1297,7 +1299,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D57">
         <v>54</v>
@@ -1492,7 +1494,7 @@
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D73">
         <v>258</v>
@@ -1510,7 +1512,7 @@
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D74">
         <v>305</v>
@@ -1528,7 +1530,7 @@
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D75">
         <v>87</v>
@@ -1546,7 +1548,7 @@
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D76">
         <v>99</v>
@@ -1573,11 +1575,10 @@
         <v>154</v>
       </c>
       <c r="F77">
-        <f>PRODUCT(D77*E77)</f>
-        <v>1540</v>
+        <v>41</v>
       </c>
       <c r="G77" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
@@ -1600,7 +1601,7 @@
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D79">
         <v>6</v>
@@ -1618,7 +1619,7 @@
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -1636,7 +1637,7 @@
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D81">
         <v>90</v>
@@ -1713,7 +1714,7 @@
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D87">
         <v>1293</v>
@@ -1731,7 +1732,7 @@
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D88">
         <v>1293</v>
@@ -1749,7 +1750,7 @@
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D89">
         <v>449</v>
@@ -1767,7 +1768,7 @@
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D90">
         <v>449</v>
@@ -1880,7 +1881,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C98" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D98">
         <v>1300</v>
@@ -1901,7 +1902,7 @@
       </c>
       <c r="B100">
         <f ca="1">SUM(F103:F148)</f>
-        <v>177609</v>
+        <v>176110</v>
       </c>
       <c r="C100" t="s">
         <v>27</v>
@@ -1986,7 +1987,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D107">
         <v>54</v>
@@ -2181,7 +2182,7 @@
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C123" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D123">
         <v>258</v>
@@ -2190,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="F123">
-        <f t="shared" ref="F123:F126" ca="1" si="13">ROUND((D123*E123)/VLOOKUP(G123, INDIRECT("K2:L3"), 2),2)</f>
+        <f t="shared" ref="F123" ca="1" si="13">ROUND((D123*E123)/VLOOKUP(G123, INDIRECT("K2:L3"), 2),2)</f>
         <v>516</v>
       </c>
       <c r="G123" t="s">
@@ -2199,7 +2200,7 @@
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C124" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D124">
         <v>305</v>
@@ -2217,7 +2218,7 @@
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C125" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D125">
         <v>87</v>
@@ -2235,7 +2236,7 @@
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C126" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D126">
         <v>99</v>
@@ -2262,11 +2263,10 @@
         <v>154</v>
       </c>
       <c r="F127">
-        <f>PRODUCT(D127*E127)</f>
-        <v>1540</v>
+        <v>41</v>
       </c>
       <c r="G127" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -2289,7 +2289,7 @@
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C129" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D129">
         <v>6</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C130" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D130">
         <v>2</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D131">
         <v>90</v>
@@ -2402,7 +2402,7 @@
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C137" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D137">
         <v>1293</v>
@@ -2420,7 +2420,7 @@
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C138" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D138">
         <v>1293</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D139">
         <v>449</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D140">
         <v>449</v>
@@ -2569,7 +2569,7 @@
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C148" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D148">
         <v>1300</v>

</xml_diff>